<commit_message>
correction d'un problème de exel
</commit_message>
<xml_diff>
--- a/data/tmp.xlsx
+++ b/data/tmp.xlsx
@@ -1303,10 +1303,10 @@
     <t>01</t>
   </si>
   <si>
-    <t>HPO001</t>
-  </si>
-  <si>
-    <t>Pompe 5.6</t>
+    <t>MOU001</t>
+  </si>
+  <si>
+    <t>Climonat XDDD</t>
   </si>
   <si>
     <t>02</t>
@@ -4670,13 +4670,13 @@
         <v>14</v>
       </c>
       <c r="E17" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="27">
-        <v>15000</v>
+        <v>500</v>
       </c>
       <c r="G17" s="27">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="H17" s="25"/>
     </row>
@@ -4975,7 +4975,7 @@
       <c r="E37" s="48"/>
       <c r="F37" s="49"/>
       <c r="G37" s="72">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="H37" s="73"/>
     </row>

</xml_diff>